<commit_message>
formatting adjustments to ALOHA data
</commit_message>
<xml_diff>
--- a/Data/AA-CSIA_ALOHA.xlsx
+++ b/Data/AA-CSIA_ALOHA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40c9661624813381/Documents/R/Organic-Matter-Supply-Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1109" documentId="13_ncr:1_{47D0C447-CF42-44CE-A2DC-F04BD3ED6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{635C8668-CAF6-4431-9BD0-870AC6BD03F3}"/>
+  <xr:revisionPtr revIDLastSave="1112" documentId="13_ncr:1_{47D0C447-CF42-44CE-A2DC-F04BD3ED6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62CC605F-A12C-46C2-8D7B-41B72955A624}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" activeTab="1" xr2:uid="{8FC557E2-921B-4618-B5F4-A9A2FDF78F4B}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" xr2:uid="{8FC557E2-921B-4618-B5F4-A9A2FDF78F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="13" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="106">
   <si>
     <t>Tow</t>
   </si>
@@ -305,16 +305,7 @@
     <t>"source" or "consumer"</t>
   </si>
   <si>
-    <t>Defines if this row containes data for an organic matter source (if so enter "source") or a consumer (if so enter "consumer").</t>
-  </si>
-  <si>
     <t>text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For sources, defines whouch organic matter source group this sample belongs to. </t>
-  </si>
-  <si>
-    <t>For consumers, just enter "consumer"</t>
   </si>
   <si>
     <t>Variable</t>
@@ -351,6 +342,21 @@
   </si>
   <si>
     <t>Bottle</t>
+  </si>
+  <si>
+    <t>Defines if this row containes data for an organic matter source or for a consumer sample.</t>
+  </si>
+  <si>
+    <t>If organic matter source, enter "Source". If consumer, enter "Consumer".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For sources, defines which organic matter source group this sample belongs to. </t>
+  </si>
+  <si>
+    <t>Source groups may also be defined programatically within the "Processing_Data" chunk. If so, leave this column blank.</t>
+  </si>
+  <si>
+    <t>For consumers, just enter "consumer".</t>
   </si>
 </sst>
 </file>
@@ -409,7 +415,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,18 +460,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -491,6 +491,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -498,7 +507,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -558,9 +567,7 @@
     <xf numFmtId="164" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -572,12 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -591,18 +592,34 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent4" xfId="2" builtinId="42"/>
@@ -681,6 +698,10 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -980,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9ACEE1-5106-4132-B432-32A94A42883E}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1003,101 +1024,117 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A2" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="51" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="53" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A4" s="54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="54" t="s">
         <v>88</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>103</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A3" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="44" t="s">
+    <row r="5" spans="1:3" s="2" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A5" s="54"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="37" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A7" s="42" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="B7" s="42" t="s">
         <v>90</v>
       </c>
+      <c r="C7" s="44" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="37" t="s">
-        <v>91</v>
-      </c>
+    <row r="8" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A8" s="43"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="45"/>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A5" s="46" t="s">
+    <row r="9" spans="1:3" s="25" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.75">
+      <c r="A9" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B9" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="48" t="s">
+      <c r="C9" s="48" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="49"/>
-    </row>
-    <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A7" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" s="50" t="s">
-        <v>96</v>
-      </c>
-      <c r="C7" s="52" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A8" s="51"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="53"/>
-    </row>
-    <row r="9" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A9" s="40" t="s">
-        <v>98</v>
-      </c>
-      <c r="B9" s="40" t="s">
-        <v>96</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="43"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="49"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.75">
-      <c r="C11" t="s">
-        <v>100</v>
+      <c r="A11" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="40" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="A12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="41"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.75">
+      <c r="C13" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="B9:B10"/>
     <mergeCell ref="C9:C10"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="B4:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1107,11 +1144,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0376732-0927-4AD5-8412-620223DD4704}">
   <dimension ref="A1:AO131"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="13" ySplit="1" topLeftCell="N121" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M138" sqref="M138"/>
+      <selection pane="bottomRight" activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -1137,7 +1174,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>44</v>
@@ -1259,7 +1296,7 @@
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A2" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>47</v>
@@ -1373,7 +1410,7 @@
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A3" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>14</v>
@@ -1475,7 +1512,7 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A4" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>14</v>
@@ -1591,7 +1628,7 @@
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A5" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>14</v>
@@ -1707,7 +1744,7 @@
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A6" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>47</v>
@@ -1823,7 +1860,7 @@
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>47</v>
@@ -1939,7 +1976,7 @@
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A8" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>47</v>
@@ -2055,7 +2092,7 @@
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -2171,7 +2208,7 @@
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A10" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>15</v>
@@ -2287,7 +2324,7 @@
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A11" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>15</v>
@@ -2404,7 +2441,7 @@
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A12" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>15</v>
@@ -2521,7 +2558,7 @@
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A13" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>15</v>
@@ -2637,7 +2674,7 @@
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A14" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>15</v>
@@ -2753,7 +2790,7 @@
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
@@ -2870,7 +2907,7 @@
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A16" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>15</v>
@@ -2987,7 +3024,7 @@
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A17" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>15</v>
@@ -3104,7 +3141,7 @@
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A18" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>47</v>
@@ -3220,7 +3257,7 @@
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A19" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>13</v>
@@ -3330,7 +3367,7 @@
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A20" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>13</v>
@@ -3434,7 +3471,7 @@
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A21" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>13</v>
@@ -3546,7 +3583,7 @@
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A22" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
@@ -3658,7 +3695,7 @@
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A23" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>13</v>
@@ -3762,7 +3799,7 @@
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A24" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
@@ -3862,7 +3899,7 @@
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A25" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>13</v>
@@ -3970,7 +4007,7 @@
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A26" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
@@ -4077,7 +4114,7 @@
         <v>17</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>45</v>
@@ -4196,7 +4233,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>45</v>
@@ -4315,7 +4352,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>45</v>
@@ -4434,7 +4471,7 @@
         <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>45</v>
@@ -4553,7 +4590,7 @@
         <v>17</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>45</v>
@@ -4672,7 +4709,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>45</v>
@@ -4791,7 +4828,7 @@
         <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>45</v>
@@ -4910,7 +4947,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>45</v>
@@ -5029,7 +5066,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>45</v>
@@ -5148,7 +5185,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>45</v>
@@ -5267,7 +5304,7 @@
         <v>17</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>45</v>
@@ -5386,7 +5423,7 @@
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>45</v>
@@ -5505,7 +5542,7 @@
         <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>45</v>
@@ -5624,7 +5661,7 @@
         <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>45</v>
@@ -5743,7 +5780,7 @@
         <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>45</v>
@@ -5862,7 +5899,7 @@
         <v>17</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>45</v>
@@ -5981,7 +6018,7 @@
         <v>17</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>45</v>
@@ -6100,7 +6137,7 @@
         <v>17</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>45</v>
@@ -6219,7 +6256,7 @@
         <v>17</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>45</v>
@@ -6338,7 +6375,7 @@
         <v>17</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>45</v>
@@ -6457,7 +6494,7 @@
         <v>17</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>45</v>
@@ -6576,7 +6613,7 @@
         <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>45</v>
@@ -6695,7 +6732,7 @@
         <v>17</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>45</v>
@@ -6810,7 +6847,7 @@
         <v>17</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>45</v>
@@ -6927,7 +6964,7 @@
         <v>17</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>45</v>
@@ -7046,7 +7083,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>45</v>
@@ -7165,7 +7202,7 @@
         <v>17</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>45</v>
@@ -7280,7 +7317,7 @@
         <v>17</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>45</v>
@@ -7395,7 +7432,7 @@
         <v>17</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>45</v>
@@ -7510,7 +7547,7 @@
         <v>17</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>45</v>
@@ -7625,7 +7662,7 @@
         <v>17</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>45</v>
@@ -7740,7 +7777,7 @@
         <v>17</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>45</v>
@@ -7855,7 +7892,7 @@
         <v>17</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>45</v>
@@ -7970,7 +8007,7 @@
         <v>17</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>45</v>
@@ -8085,7 +8122,7 @@
         <v>17</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>45</v>
@@ -8200,7 +8237,7 @@
         <v>17</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>45</v>
@@ -8315,7 +8352,7 @@
         <v>17</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>45</v>
@@ -8432,7 +8469,7 @@
         <v>17</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>45</v>
@@ -8548,7 +8585,7 @@
     </row>
     <row r="65" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A65" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>47</v>
@@ -8660,7 +8697,7 @@
     </row>
     <row r="66" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A66" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>14</v>
@@ -8776,7 +8813,7 @@
     </row>
     <row r="67" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A67" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>14</v>
@@ -8892,7 +8929,7 @@
     </row>
     <row r="68" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A68" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>14</v>
@@ -9008,7 +9045,7 @@
     </row>
     <row r="69" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A69" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>47</v>
@@ -9124,7 +9161,7 @@
     </row>
     <row r="70" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A70" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>47</v>
@@ -9240,7 +9277,7 @@
     </row>
     <row r="71" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A71" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>47</v>
@@ -9356,7 +9393,7 @@
     </row>
     <row r="72" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A72" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>15</v>
@@ -9472,7 +9509,7 @@
     </row>
     <row r="73" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A73" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>15</v>
@@ -9588,7 +9625,7 @@
     </row>
     <row r="74" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A74" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>15</v>
@@ -9701,7 +9738,7 @@
     </row>
     <row r="75" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A75" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>15</v>
@@ -9818,7 +9855,7 @@
     </row>
     <row r="76" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A76" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>15</v>
@@ -9934,7 +9971,7 @@
     </row>
     <row r="77" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A77" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>15</v>
@@ -10050,7 +10087,7 @@
     </row>
     <row r="78" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A78" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>15</v>
@@ -10167,7 +10204,7 @@
     </row>
     <row r="79" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A79" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>15</v>
@@ -10284,7 +10321,7 @@
     </row>
     <row r="80" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A80" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>15</v>
@@ -10401,7 +10438,7 @@
     </row>
     <row r="81" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A81" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>47</v>
@@ -10517,7 +10554,7 @@
     </row>
     <row r="82" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A82" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>13</v>
@@ -10629,7 +10666,7 @@
     </row>
     <row r="83" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A83" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>13</v>
@@ -10745,7 +10782,7 @@
     </row>
     <row r="84" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A84" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>13</v>
@@ -10857,7 +10894,7 @@
     </row>
     <row r="85" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A85" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>13</v>
@@ -10969,7 +11006,7 @@
     </row>
     <row r="86" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A86" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>13</v>
@@ -11081,7 +11118,7 @@
     </row>
     <row r="87" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A87" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>13</v>
@@ -11193,10 +11230,10 @@
     </row>
     <row r="88" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A88" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>78</v>
@@ -11296,10 +11333,10 @@
     </row>
     <row r="89" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A89" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>78</v>
@@ -11415,10 +11452,10 @@
     </row>
     <row r="90" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A90" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>78</v>
@@ -11534,10 +11571,10 @@
     </row>
     <row r="91" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A91" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>78</v>
@@ -11653,10 +11690,10 @@
     </row>
     <row r="92" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A92" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>78</v>
@@ -11772,10 +11809,10 @@
     </row>
     <row r="93" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A93" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>78</v>
@@ -11891,10 +11928,10 @@
     </row>
     <row r="94" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A94" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>78</v>
@@ -12010,10 +12047,10 @@
     </row>
     <row r="95" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A95" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>78</v>
@@ -12129,10 +12166,10 @@
     </row>
     <row r="96" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A96" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>78</v>
@@ -12248,10 +12285,10 @@
     </row>
     <row r="97" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A97" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>78</v>
@@ -12367,10 +12404,10 @@
     </row>
     <row r="98" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A98" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>78</v>
@@ -12486,10 +12523,10 @@
     </row>
     <row r="99" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A99" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>78</v>
@@ -12605,10 +12642,10 @@
     </row>
     <row r="100" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A100" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>78</v>
@@ -12724,10 +12761,10 @@
     </row>
     <row r="101" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A101" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>78</v>
@@ -12843,10 +12880,10 @@
     </row>
     <row r="102" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A102" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>78</v>
@@ -12962,10 +12999,10 @@
     </row>
     <row r="103" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A103" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>78</v>
@@ -13081,10 +13118,10 @@
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A104" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>78</v>
@@ -13200,10 +13237,10 @@
     </row>
     <row r="105" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A105" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>78</v>
@@ -13319,10 +13356,10 @@
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A106" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>78</v>
@@ -13438,10 +13475,10 @@
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A107" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>78</v>
@@ -13557,10 +13594,10 @@
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A108" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>78</v>
@@ -13676,10 +13713,10 @@
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A109" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>78</v>
@@ -13788,10 +13825,10 @@
     </row>
     <row r="110" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A110" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>78</v>
@@ -13882,10 +13919,10 @@
     </row>
     <row r="111" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A111" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>78</v>
@@ -13982,10 +14019,10 @@
     </row>
     <row r="112" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A112" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>78</v>
@@ -14094,10 +14131,10 @@
     </row>
     <row r="113" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A113" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>78</v>
@@ -14210,10 +14247,10 @@
     </row>
     <row r="114" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A114" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>78</v>
@@ -14322,10 +14359,10 @@
     </row>
     <row r="115" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A115" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>78</v>
@@ -14434,10 +14471,10 @@
     </row>
     <row r="116" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A116" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>78</v>
@@ -14546,10 +14583,10 @@
     </row>
     <row r="117" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A117" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>78</v>
@@ -14658,10 +14695,10 @@
     </row>
     <row r="118" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A118" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>78</v>
@@ -14770,10 +14807,10 @@
     </row>
     <row r="119" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A119" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>78</v>
@@ -14882,10 +14919,10 @@
     </row>
     <row r="120" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A120" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>78</v>
@@ -14994,10 +15031,10 @@
     </row>
     <row r="121" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A121" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C121" s="4" t="s">
         <v>78</v>
@@ -15106,7 +15143,7 @@
     </row>
     <row r="122" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A122" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>81</v>
@@ -15118,7 +15155,7 @@
         <v>79</v>
       </c>
       <c r="F122" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H122" s="4">
         <v>7.5</v>
@@ -15201,7 +15238,7 @@
     </row>
     <row r="123" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A123" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>81</v>
@@ -15213,7 +15250,7 @@
         <v>79</v>
       </c>
       <c r="F123" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H123" s="4">
         <v>7.5</v>
@@ -15296,7 +15333,7 @@
     </row>
     <row r="124" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A124" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>81</v>
@@ -15308,7 +15345,7 @@
         <v>79</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H124" s="4">
         <v>400</v>
@@ -15391,7 +15428,7 @@
     </row>
     <row r="125" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A125" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>81</v>
@@ -15403,7 +15440,7 @@
         <v>79</v>
       </c>
       <c r="F125" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H125" s="4">
         <v>850</v>
@@ -15489,7 +15526,7 @@
     </row>
     <row r="126" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A126" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>81</v>
@@ -15501,7 +15538,7 @@
         <v>79</v>
       </c>
       <c r="F126" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H126" s="4">
         <v>2500</v>
@@ -15578,7 +15615,7 @@
     </row>
     <row r="127" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A127" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>81</v>
@@ -15590,7 +15627,7 @@
         <v>79</v>
       </c>
       <c r="F127" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H127" s="4">
         <v>7.5</v>
@@ -15673,7 +15710,7 @@
     </row>
     <row r="128" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A128" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>81</v>
@@ -15685,7 +15722,7 @@
         <v>79</v>
       </c>
       <c r="F128" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H128" s="4">
         <v>7.5</v>
@@ -15762,7 +15799,7 @@
     </row>
     <row r="129" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A129" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>81</v>
@@ -15774,7 +15811,7 @@
         <v>79</v>
       </c>
       <c r="F129" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H129" s="4">
         <v>400</v>
@@ -15863,7 +15900,7 @@
     </row>
     <row r="130" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A130" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>81</v>
@@ -15875,7 +15912,7 @@
         <v>79</v>
       </c>
       <c r="F130" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H130" s="4">
         <v>850</v>
@@ -15964,7 +16001,7 @@
     </row>
     <row r="131" spans="1:41" x14ac:dyDescent="0.75">
       <c r="A131" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>81</v>
@@ -15976,7 +16013,7 @@
         <v>79</v>
       </c>
       <c r="F131" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H131" s="4">
         <v>2500</v>

</xml_diff>